<commit_message>
Backlog | Chart Refresh
Refresh of the Excel Backlog and Chart
</commit_message>
<xml_diff>
--- a/Gehweg-Parcours Product Backlog.xlsx
+++ b/Gehweg-Parcours Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive\Schule\Klasse 11\IT\Software\eclipse\Gehweg-Parcours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\@Warum\Workspace_Kaunas_Adrian\Gehweg-Parcours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EB2892-F5C1-4961-92EE-C61BB4420A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5CA1F2-151A-4D67-9BDF-3E58BE3BDA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5BE05EE6-96E2-45D5-9F22-0F39015F8532}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="13080" xr2:uid="{5BE05EE6-96E2-45D5-9F22-0F39015F8532}"/>
   </bookViews>
   <sheets>
     <sheet name="Gehweg-Parcours" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>Bearbeiter</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Eingabefeld</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -733,29 +736,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCECBA3-BFA8-47EE-AA9B-3B26E808E77B}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.46484375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.77734375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="25.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.796875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="25.796875" style="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.19921875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="10.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.46484375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -796,7 +799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>56</v>
       </c>
@@ -819,7 +822,7 @@
       <c r="L2" s="20"/>
       <c r="M2" s="20"/>
     </row>
-    <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -843,7 +846,7 @@
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
     </row>
-    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>30</v>
       </c>
@@ -870,9 +873,11 @@
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M4" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
@@ -899,9 +904,11 @@
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M5" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -925,7 +932,7 @@
       <c r="L6" s="23"/>
       <c r="M6" s="23"/>
     </row>
-    <row r="7" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>33</v>
       </c>
@@ -952,9 +959,11 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M7" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>35</v>
       </c>
@@ -981,9 +990,11 @@
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="M8" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1008,9 +1019,11 @@
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M9" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
@@ -1034,7 +1047,7 @@
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
     </row>
-    <row r="11" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>38</v>
       </c>
@@ -1061,9 +1074,11 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M11" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -1088,9 +1103,11 @@
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M12" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
@@ -1115,9 +1132,11 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M13" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>36</v>
       </c>
@@ -1144,9 +1163,11 @@
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M14" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>41</v>
       </c>
@@ -1171,9 +1192,11 @@
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M15" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -1197,7 +1220,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="23"/>
     </row>
-    <row r="17" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>47</v>
       </c>
@@ -1219,12 +1242,14 @@
       <c r="G17" s="15"/>
       <c r="H17" s="16"/>
       <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
@@ -1248,7 +1273,7 @@
       <c r="L18" s="23"/>
       <c r="M18" s="23"/>
     </row>
-    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>49</v>
       </c>
@@ -1273,9 +1298,11 @@
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M19" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>42</v>
       </c>
@@ -1297,12 +1324,14 @@
       <c r="G20" s="15"/>
       <c r="H20" s="16"/>
       <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
       <c r="M20" s="14"/>
     </row>
-    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
@@ -1326,7 +1355,7 @@
       <c r="L21" s="23"/>
       <c r="M21" s="23"/>
     </row>
-    <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>44</v>
       </c>
@@ -1350,12 +1379,14 @@
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="J22" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
       <c r="M22" s="14"/>
     </row>
-    <row r="23" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>45</v>
       </c>
@@ -1379,7 +1410,9 @@
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+      <c r="J23" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>

</xml_diff>